<commit_message>
add some more take down info
</commit_message>
<xml_diff>
--- a/Data/Raw/Camera_info.xlsx
+++ b/Data/Raw/Camera_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Library/Mobile Documents/com~apple~CloudDocs/Documents/University/PhD/Data/Gosforth_mammals/Data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Library/Mobile Documents/com~apple~CloudDocs/Documents/University/PhD/Data/Gosforth_mammals/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F1D91-999F-B143-9D5E-C28B3C4B9727}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8732E2C-F88F-0849-A623-EF579632EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16620" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
+    <workbookView xWindow="7500" yWindow="500" windowWidth="20920" windowHeight="17500" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>031</t>
   </si>
   <si>
-    <t>041</t>
-  </si>
-  <si>
     <t>Scots Pine</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Date_in</t>
+  </si>
+  <si>
+    <t>041 (or 42?)</t>
   </si>
 </sst>
 </file>
@@ -183,12 +183,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -203,11 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +533,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,31 +555,31 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
       <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
         <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
       <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
         <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -759,11 +767,19 @@
       <c r="E7" s="2">
         <v>44074</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="3">
+        <v>44421</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
         <v>20</v>
+      </c>
+      <c r="L7" s="5">
+        <v>10</v>
+      </c>
+      <c r="M7" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -788,6 +804,8 @@
       <c r="I8" t="s">
         <v>22</v>
       </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -846,6 +864,8 @@
       <c r="I10" t="s">
         <v>22</v>
       </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -863,11 +883,19 @@
       <c r="E11" s="2">
         <v>44075</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3">
+        <v>44421</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
         <v>27</v>
+      </c>
+      <c r="L11" s="5">
+        <v>10</v>
+      </c>
+      <c r="M11" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -892,6 +920,8 @@
       <c r="I12" t="s">
         <v>22</v>
       </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -939,7 +969,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2">
         <v>44076</v>
@@ -950,6 +980,8 @@
       <c r="I14" t="s">
         <v>22</v>
       </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -962,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2">
         <v>44077</v>
@@ -977,7 +1009,7 @@
         <v>44123</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L15">
         <v>12</v>
@@ -1067,7 +1099,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="2">
         <v>44092</v>
@@ -1102,7 +1134,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" s="2">
         <v>44092</v>

</xml_diff>

<commit_message>
added image start and end dates from cards 83, 55, 84, 41 and 17
</commit_message>
<xml_diff>
--- a/Data/Raw/Camera_info.xlsx
+++ b/Data/Raw/Camera_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Library/Mobile Documents/com~apple~CloudDocs/Documents/University/PhD/Data/Gosforth_mammals/Data/Raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Gosforth_mammals/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8732E2C-F88F-0849-A623-EF579632EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{A8732E2C-F88F-0849-A623-EF579632EB3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC9986A-264B-496A-96CE-F6235EED5421}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="500" windowWidth="20920" windowHeight="17500" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Point_ID</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>041 (or 42?)</t>
+  </si>
+  <si>
+    <t>084?</t>
   </si>
 </sst>
 </file>
@@ -533,15 +536,15 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -611,7 +614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -646,7 +649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -681,7 +684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -716,7 +719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -751,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -770,8 +773,12 @@
       <c r="F7" s="3">
         <v>44421</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2">
+        <v>44074</v>
+      </c>
+      <c r="H7" s="2">
+        <v>44421</v>
+      </c>
       <c r="I7" t="s">
         <v>20</v>
       </c>
@@ -782,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -793,21 +800,27 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2">
         <v>44074</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="2">
+        <v>44421</v>
+      </c>
+      <c r="G8" s="2">
+        <v>42735</v>
+      </c>
+      <c r="H8" s="2">
+        <v>42735</v>
+      </c>
       <c r="I8" t="s">
         <v>22</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -842,7 +855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -867,7 +880,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -886,8 +899,12 @@
       <c r="F11" s="3">
         <v>44421</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2">
+        <v>44075</v>
+      </c>
+      <c r="H11" s="2">
+        <v>42737</v>
+      </c>
       <c r="I11" t="s">
         <v>27</v>
       </c>
@@ -898,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -914,16 +931,22 @@
       <c r="E12" s="2">
         <v>44076</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="3">
+        <v>44421</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44076</v>
+      </c>
+      <c r="H12" s="2">
+        <v>42775</v>
+      </c>
       <c r="I12" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -958,7 +981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -974,16 +997,22 @@
       <c r="E14" s="2">
         <v>44076</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="2">
+        <v>44421</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44076</v>
+      </c>
+      <c r="H14" s="2">
+        <v>44083</v>
+      </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1018,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1053,7 +1082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1088,7 +1117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1123,7 +1152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1158,7 +1187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1195,5 +1224,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>